<commit_message>
start working on making therapy date week 0. will need to make injury date week 0 instead, and separate stim and no stim groups
</commit_message>
<xml_diff>
--- a/Rat Review.xlsx
+++ b/Rat Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathuser/Documents/Perl Lab Rat Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ED271BC1-DDB1-9B40-BF40-D1F007F6DCE6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{96305A72-3545-AA42-B15D-2EDC47ED5045}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="460" windowWidth="23400" windowHeight="15000" xr2:uid="{492C9695-63A7-E247-8A26-3C145580BC5E}"/>
+    <workbookView xWindow="12520" yWindow="460" windowWidth="13000" windowHeight="15000" xr2:uid="{492C9695-63A7-E247-8A26-3C145580BC5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC0818A-4301-F542-9C62-BCE947E9F3B7}">
   <dimension ref="A1:AY29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="AS18" sqref="AS18"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="AX14" sqref="AX14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,6 +773,46 @@
       <c r="AI4">
         <v>1</v>
       </c>
+      <c r="AK4" s="1">
+        <v>43332</v>
+      </c>
+      <c r="AL4" s="8">
+        <f t="shared" ref="AL4:AL27" si="4">ROUNDDOWN((AK4-43332)/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>34</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>43332</v>
+      </c>
+      <c r="AP4" s="8">
+        <f t="shared" ref="AP4:AP7" si="5">ROUNDDOWN((AO4-43332)/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>29</v>
+      </c>
+      <c r="AS4" s="1">
+        <v>43332</v>
+      </c>
+      <c r="AT4" s="8">
+        <f t="shared" ref="AT4:AT26" si="6">ROUNDDOWN((AS4-43332)/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>38</v>
+      </c>
+      <c r="AW4" s="1">
+        <v>43332</v>
+      </c>
+      <c r="AX4" s="8">
+        <f t="shared" ref="AX4:AX26" si="7">ROUNDDOWN((AW4-43332)/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -836,13 +876,53 @@
       <c r="AI5">
         <v>0</v>
       </c>
+      <c r="AK5" s="1">
+        <v>43333</v>
+      </c>
+      <c r="AL5" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>30</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>43333</v>
+      </c>
+      <c r="AP5" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>34</v>
+      </c>
+      <c r="AS5" s="1">
+        <v>43333</v>
+      </c>
+      <c r="AT5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>30</v>
+      </c>
+      <c r="AW5" s="1">
+        <v>43333</v>
+      </c>
+      <c r="AX5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43271</v>
       </c>
       <c r="B6" s="8">
-        <f t="shared" ref="B6:B9" si="4">ROUNDDOWN((A6-43270)/5,0)</f>
+        <f t="shared" ref="B6:B9" si="8">ROUNDDOWN((A6-43270)/5,0)</f>
         <v>0</v>
       </c>
       <c r="C6">
@@ -852,7 +932,7 @@
         <v>43271</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F27" si="5">ROUNDDOWN((E6-43270)/5,0)</f>
+        <f t="shared" ref="F6:F27" si="9">ROUNDDOWN((E6-43270)/5,0)</f>
         <v>0</v>
       </c>
       <c r="G6">
@@ -927,6 +1007,46 @@
       </c>
       <c r="AI6">
         <v>0</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>43334</v>
+      </c>
+      <c r="AL6" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>37</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>43334</v>
+      </c>
+      <c r="AP6" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>31</v>
+      </c>
+      <c r="AS6" s="1">
+        <v>43334</v>
+      </c>
+      <c r="AT6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>30</v>
+      </c>
+      <c r="AW6" s="1">
+        <v>43334</v>
+      </c>
+      <c r="AX6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.2">
@@ -934,7 +1054,7 @@
         <v>43272</v>
       </c>
       <c r="B7" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C7">
@@ -944,7 +1064,7 @@
         <v>43272</v>
       </c>
       <c r="F7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G7">
@@ -954,7 +1074,7 @@
         <v>43272</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J26" si="6">ROUNDDOWN((I7-43271)/5,0)</f>
+        <f t="shared" ref="J7:J26" si="10">ROUNDDOWN((I7-43271)/5,0)</f>
         <v>0</v>
       </c>
       <c r="K7">
@@ -964,7 +1084,7 @@
         <v>43272</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N26" si="7">ROUNDDOWN((M7-43271)/5,0)</f>
+        <f t="shared" ref="N7:N26" si="11">ROUNDDOWN((M7-43271)/5,0)</f>
         <v>0</v>
       </c>
       <c r="O7">
@@ -974,7 +1094,7 @@
         <v>43272</v>
       </c>
       <c r="R7">
-        <f t="shared" ref="R7:R26" si="8">ROUNDDOWN((Q7-43271)/5,0)</f>
+        <f t="shared" ref="R7:R26" si="12">ROUNDDOWN((Q7-43271)/5,0)</f>
         <v>0</v>
       </c>
       <c r="S7" s="7">
@@ -1024,8 +1144,8 @@
         <v>43339</v>
       </c>
       <c r="AL7" s="8">
-        <f>ROUNDDOWN((AK7-43339)/5,0)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="AM7">
         <v>33</v>
@@ -1034,8 +1154,8 @@
         <v>43339</v>
       </c>
       <c r="AP7" s="8">
-        <f>ROUNDDOWN((AO7-43339)/5,0)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="AQ7">
         <v>35</v>
@@ -1044,8 +1164,8 @@
         <v>43339</v>
       </c>
       <c r="AT7" s="8">
-        <f>ROUNDDOWN((AS7-43339)/5,0)</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AU7">
         <v>30</v>
@@ -1054,8 +1174,8 @@
         <v>43339</v>
       </c>
       <c r="AX7" s="8">
-        <f>ROUNDDOWN((AW7-43339)/5,0)</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="AY7">
         <v>40</v>
@@ -1066,35 +1186,35 @@
         <v>43277</v>
       </c>
       <c r="B8" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="E8" s="4">
         <v>43277</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I8" s="4">
         <v>43277</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="M8" s="4">
         <v>43277</v>
       </c>
       <c r="N8" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="Q8" s="4">
         <v>43277</v>
       </c>
       <c r="R8" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="U8" s="4">
@@ -1132,29 +1252,29 @@
         <v>43340</v>
       </c>
       <c r="AL8" s="5">
-        <f t="shared" ref="AL8:AL27" si="9">ROUNDDOWN((AK8-43339)/5,0)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="AO8" s="4">
         <v>43340</v>
       </c>
       <c r="AP8" s="5">
-        <f t="shared" ref="AP8:AP27" si="10">ROUNDDOWN((AO8-43339)/5,0)</f>
-        <v>0</v>
+        <f t="shared" ref="AP8:AP27" si="13">ROUNDDOWN((AO8-43332)/5,0)</f>
+        <v>1</v>
       </c>
       <c r="AS8" s="4">
         <v>43340</v>
       </c>
       <c r="AT8" s="5">
-        <f t="shared" ref="AT8:AT27" si="11">ROUNDDOWN((AS8-43339)/5,0)</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AW8" s="4">
         <v>43340</v>
       </c>
       <c r="AX8" s="5">
-        <f t="shared" ref="AX8:AX27" si="12">ROUNDDOWN((AW8-43339)/5,0)</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.2">
@@ -1162,7 +1282,7 @@
         <v>43290</v>
       </c>
       <c r="B9" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="C9">
@@ -1172,7 +1292,7 @@
         <v>43290</v>
       </c>
       <c r="F9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="G9">
@@ -1182,7 +1302,7 @@
         <v>43290</v>
       </c>
       <c r="J9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="K9">
@@ -1192,7 +1312,7 @@
         <v>43290</v>
       </c>
       <c r="N9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="O9">
@@ -1202,7 +1322,7 @@
         <v>43290</v>
       </c>
       <c r="R9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="S9">
@@ -1222,8 +1342,8 @@
         <v>43353</v>
       </c>
       <c r="AL9">
-        <f t="shared" si="9"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="AM9">
         <v>12</v>
@@ -1231,9 +1351,9 @@
       <c r="AO9" s="1">
         <v>43353</v>
       </c>
-      <c r="AP9">
-        <f t="shared" si="10"/>
-        <v>2</v>
+      <c r="AP9" s="8">
+        <f t="shared" si="13"/>
+        <v>4</v>
       </c>
       <c r="AQ9">
         <v>4</v>
@@ -1242,8 +1362,8 @@
         <v>43353</v>
       </c>
       <c r="AT9">
-        <f t="shared" si="11"/>
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="AU9">
         <v>7</v>
@@ -1252,8 +1372,8 @@
         <v>43353</v>
       </c>
       <c r="AX9">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="AY9">
         <v>0</v>
@@ -1264,7 +1384,7 @@
         <v>43292</v>
       </c>
       <c r="F10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="G10">
@@ -1274,7 +1394,7 @@
         <v>43291</v>
       </c>
       <c r="J10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="K10">
@@ -1284,7 +1404,7 @@
         <v>43292</v>
       </c>
       <c r="N10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="O10">
@@ -1294,7 +1414,7 @@
         <v>43293</v>
       </c>
       <c r="R10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="S10">
@@ -1344,8 +1464,8 @@
         <v>43361</v>
       </c>
       <c r="AL10">
-        <f t="shared" si="9"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="AM10">
         <v>17</v>
@@ -1353,9 +1473,9 @@
       <c r="AO10" s="1">
         <v>43361</v>
       </c>
-      <c r="AP10">
-        <f t="shared" si="10"/>
-        <v>4</v>
+      <c r="AP10" s="8">
+        <f t="shared" si="13"/>
+        <v>5</v>
       </c>
       <c r="AQ10">
         <v>2</v>
@@ -1364,8 +1484,8 @@
         <v>43361</v>
       </c>
       <c r="AT10">
-        <f t="shared" si="11"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="AU10">
         <v>3</v>
@@ -1374,8 +1494,8 @@
         <v>43361</v>
       </c>
       <c r="AX10">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="7"/>
+        <v>5</v>
       </c>
       <c r="AY10">
         <v>3</v>
@@ -1386,7 +1506,7 @@
         <v>43293</v>
       </c>
       <c r="J11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="K11">
@@ -1436,8 +1556,8 @@
         <v>43362</v>
       </c>
       <c r="AL11">
-        <f t="shared" si="9"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="AM11">
         <v>20</v>
@@ -1445,9 +1565,9 @@
       <c r="AO11" s="1">
         <v>43362</v>
       </c>
-      <c r="AP11">
-        <f t="shared" si="10"/>
-        <v>4</v>
+      <c r="AP11" s="8">
+        <f t="shared" si="13"/>
+        <v>6</v>
       </c>
       <c r="AQ11">
         <v>1</v>
@@ -1456,8 +1576,8 @@
         <v>43362</v>
       </c>
       <c r="AT11">
-        <f t="shared" si="11"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="AU11">
         <v>2</v>
@@ -1466,8 +1586,8 @@
         <v>43362</v>
       </c>
       <c r="AX11">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="7"/>
+        <v>6</v>
       </c>
       <c r="AY11">
         <v>5</v>
@@ -1478,7 +1598,7 @@
         <v>43297</v>
       </c>
       <c r="F12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="G12">
@@ -1488,7 +1608,7 @@
         <v>43297</v>
       </c>
       <c r="J12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="K12">
@@ -1498,7 +1618,7 @@
         <v>43297</v>
       </c>
       <c r="N12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O12">
@@ -1508,7 +1628,7 @@
         <v>43297</v>
       </c>
       <c r="R12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="S12">
@@ -1558,8 +1678,8 @@
         <v>43363</v>
       </c>
       <c r="AL12">
-        <f t="shared" si="9"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="AM12">
         <v>21</v>
@@ -1567,9 +1687,9 @@
       <c r="AO12" s="1">
         <v>43363</v>
       </c>
-      <c r="AP12">
-        <f t="shared" si="10"/>
-        <v>4</v>
+      <c r="AP12" s="8">
+        <f t="shared" si="13"/>
+        <v>6</v>
       </c>
       <c r="AQ12">
         <v>1</v>
@@ -1578,8 +1698,8 @@
         <v>43363</v>
       </c>
       <c r="AT12">
-        <f t="shared" si="11"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="AU12">
         <v>5</v>
@@ -1588,8 +1708,8 @@
         <v>43363</v>
       </c>
       <c r="AX12">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="7"/>
+        <v>6</v>
       </c>
       <c r="AY12">
         <v>10</v>
@@ -1600,7 +1720,7 @@
         <v>43298</v>
       </c>
       <c r="F13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="G13">
@@ -1610,7 +1730,7 @@
         <v>43298</v>
       </c>
       <c r="J13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="K13">
@@ -1620,7 +1740,7 @@
         <v>43298</v>
       </c>
       <c r="N13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O13">
@@ -1630,7 +1750,7 @@
         <v>43298</v>
       </c>
       <c r="R13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="S13">
@@ -1680,8 +1800,8 @@
         <v>43364</v>
       </c>
       <c r="AL13">
-        <f t="shared" si="9"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="AM13">
         <v>15</v>
@@ -1689,9 +1809,9 @@
       <c r="AO13" s="1">
         <v>43364</v>
       </c>
-      <c r="AP13">
-        <f t="shared" si="10"/>
-        <v>5</v>
+      <c r="AP13" s="8">
+        <f t="shared" si="13"/>
+        <v>6</v>
       </c>
       <c r="AQ13">
         <v>2</v>
@@ -1700,8 +1820,8 @@
         <v>43364</v>
       </c>
       <c r="AT13">
-        <f t="shared" si="11"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="AU13">
         <v>8</v>
@@ -1710,8 +1830,8 @@
         <v>43364</v>
       </c>
       <c r="AX13">
-        <f t="shared" si="12"/>
-        <v>5</v>
+        <f t="shared" si="7"/>
+        <v>6</v>
       </c>
       <c r="AY13">
         <v>6</v>
@@ -1722,7 +1842,7 @@
         <v>43299</v>
       </c>
       <c r="F14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="G14">
@@ -1732,7 +1852,7 @@
         <v>43299</v>
       </c>
       <c r="J14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="K14">
@@ -1742,7 +1862,7 @@
         <v>43299</v>
       </c>
       <c r="N14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O14">
@@ -1752,7 +1872,7 @@
         <v>43299</v>
       </c>
       <c r="R14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="S14">
@@ -1798,6 +1918,7 @@
       <c r="AI14">
         <v>0</v>
       </c>
+      <c r="AP14" s="8"/>
       <c r="AW14" s="1"/>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.2">
@@ -1805,7 +1926,7 @@
         <v>43300</v>
       </c>
       <c r="F15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="G15">
@@ -1815,7 +1936,7 @@
         <v>43300</v>
       </c>
       <c r="J15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="K15">
@@ -1825,7 +1946,7 @@
         <v>43300</v>
       </c>
       <c r="N15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O15">
@@ -1835,7 +1956,7 @@
         <v>43300</v>
       </c>
       <c r="R15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="S15">
@@ -1881,6 +2002,7 @@
       <c r="AI15">
         <v>0</v>
       </c>
+      <c r="AP15" s="8"/>
       <c r="AW15" s="1"/>
     </row>
     <row r="16" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1892,7 +2014,7 @@
         <v>43301</v>
       </c>
       <c r="F16" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="G16" s="11">
@@ -1903,7 +2025,7 @@
         <v>43301</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="K16" s="3">
@@ -1914,7 +2036,7 @@
         <v>43301</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O16" s="3">
@@ -1925,7 +2047,7 @@
         <v>43301</v>
       </c>
       <c r="R16" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="S16" s="11">
@@ -1980,8 +2102,8 @@
         <v>43367</v>
       </c>
       <c r="AL16" s="11">
-        <f t="shared" si="9"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7</v>
       </c>
       <c r="AM16" s="11">
         <v>14</v>
@@ -1991,8 +2113,8 @@
         <v>43367</v>
       </c>
       <c r="AP16" s="3">
-        <f t="shared" si="10"/>
-        <v>5</v>
+        <f t="shared" si="13"/>
+        <v>7</v>
       </c>
       <c r="AQ16" s="3">
         <v>3</v>
@@ -2001,8 +2123,8 @@
         <v>43367</v>
       </c>
       <c r="AT16" s="3">
-        <f t="shared" si="11"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="AU16" s="3">
         <v>10</v>
@@ -2011,8 +2133,8 @@
         <v>43367</v>
       </c>
       <c r="AX16" s="3">
-        <f t="shared" si="12"/>
-        <v>5</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="AY16" s="3">
         <v>2</v>
@@ -2023,7 +2145,7 @@
         <v>43304</v>
       </c>
       <c r="F17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="G17">
@@ -2033,7 +2155,7 @@
         <v>43304</v>
       </c>
       <c r="J17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="K17">
@@ -2043,7 +2165,7 @@
         <v>43304</v>
       </c>
       <c r="N17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O17">
@@ -2053,7 +2175,7 @@
         <v>43304</v>
       </c>
       <c r="R17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="S17">
@@ -2103,8 +2225,8 @@
         <v>43368</v>
       </c>
       <c r="AL17">
-        <f t="shared" si="9"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7</v>
       </c>
       <c r="AM17">
         <v>17</v>
@@ -2112,9 +2234,9 @@
       <c r="AO17" s="1">
         <v>43368</v>
       </c>
-      <c r="AP17">
-        <f t="shared" si="10"/>
-        <v>5</v>
+      <c r="AP17" s="8">
+        <f t="shared" si="13"/>
+        <v>7</v>
       </c>
       <c r="AQ17">
         <v>1</v>
@@ -2123,8 +2245,8 @@
         <v>43368</v>
       </c>
       <c r="AT17">
-        <f t="shared" si="11"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="AU17">
         <v>13</v>
@@ -2133,8 +2255,8 @@
         <v>43368</v>
       </c>
       <c r="AX17">
-        <f t="shared" si="12"/>
-        <v>5</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="AY17">
         <v>0</v>
@@ -2145,7 +2267,7 @@
         <v>43305</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="G18">
@@ -2155,7 +2277,7 @@
         <v>43305</v>
       </c>
       <c r="J18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="K18">
@@ -2165,7 +2287,7 @@
         <v>43305</v>
       </c>
       <c r="N18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="O18">
@@ -2175,7 +2297,7 @@
         <v>43305</v>
       </c>
       <c r="R18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="S18">
@@ -2225,8 +2347,8 @@
         <v>43369</v>
       </c>
       <c r="AL18">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>7</v>
       </c>
       <c r="AM18">
         <v>19</v>
@@ -2234,9 +2356,9 @@
       <c r="AO18" s="1">
         <v>43369</v>
       </c>
-      <c r="AP18">
-        <f t="shared" si="10"/>
-        <v>6</v>
+      <c r="AP18" s="8">
+        <f t="shared" si="13"/>
+        <v>7</v>
       </c>
       <c r="AQ18">
         <v>5</v>
@@ -2245,8 +2367,8 @@
         <v>43369</v>
       </c>
       <c r="AT18">
-        <f t="shared" si="11"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="AU18">
         <v>0</v>
@@ -2255,8 +2377,8 @@
         <v>43369</v>
       </c>
       <c r="AX18">
-        <f t="shared" si="12"/>
-        <v>6</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="AY18">
         <v>7</v>
@@ -2267,7 +2389,7 @@
         <v>43306</v>
       </c>
       <c r="F19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="G19">
@@ -2277,7 +2399,7 @@
         <v>43306</v>
       </c>
       <c r="J19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="K19">
@@ -2287,7 +2409,7 @@
         <v>43306</v>
       </c>
       <c r="N19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O19">
@@ -2297,7 +2419,7 @@
         <v>43306</v>
       </c>
       <c r="R19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="S19">
@@ -2347,8 +2469,8 @@
         <v>43370</v>
       </c>
       <c r="AL19">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>7</v>
       </c>
       <c r="AM19">
         <v>24</v>
@@ -2356,9 +2478,9 @@
       <c r="AO19" s="1">
         <v>43370</v>
       </c>
-      <c r="AP19">
-        <f t="shared" si="10"/>
-        <v>6</v>
+      <c r="AP19" s="8">
+        <f t="shared" si="13"/>
+        <v>7</v>
       </c>
       <c r="AQ19">
         <v>10</v>
@@ -2367,8 +2489,8 @@
         <v>43370</v>
       </c>
       <c r="AT19">
-        <f t="shared" si="11"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="AU19">
         <v>10</v>
@@ -2377,8 +2499,8 @@
         <v>43370</v>
       </c>
       <c r="AX19">
-        <f t="shared" si="12"/>
-        <v>6</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="AY19">
         <v>9</v>
@@ -2389,7 +2511,7 @@
         <v>43307</v>
       </c>
       <c r="F20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="G20">
@@ -2399,7 +2521,7 @@
         <v>43307</v>
       </c>
       <c r="J20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="K20">
@@ -2409,7 +2531,7 @@
         <v>43307</v>
       </c>
       <c r="N20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O20">
@@ -2419,7 +2541,7 @@
         <v>43307</v>
       </c>
       <c r="R20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="S20">
@@ -2469,8 +2591,8 @@
         <v>43371</v>
       </c>
       <c r="AL20">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>7</v>
       </c>
       <c r="AM20">
         <v>19</v>
@@ -2478,9 +2600,9 @@
       <c r="AO20" s="1">
         <v>43371</v>
       </c>
-      <c r="AP20">
-        <f t="shared" si="10"/>
-        <v>6</v>
+      <c r="AP20" s="8">
+        <f t="shared" si="13"/>
+        <v>7</v>
       </c>
       <c r="AQ20">
         <v>6</v>
@@ -2489,8 +2611,8 @@
         <v>43371</v>
       </c>
       <c r="AT20">
-        <f t="shared" si="11"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="AU20">
         <v>7</v>
@@ -2499,8 +2621,8 @@
         <v>43371</v>
       </c>
       <c r="AX20">
-        <f t="shared" si="12"/>
-        <v>6</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="AY20">
         <v>5</v>
@@ -2511,7 +2633,7 @@
         <v>43308</v>
       </c>
       <c r="F21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="G21">
@@ -2521,7 +2643,7 @@
         <v>43308</v>
       </c>
       <c r="J21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="K21">
@@ -2531,7 +2653,7 @@
         <v>43308</v>
       </c>
       <c r="N21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="O21">
@@ -2541,7 +2663,7 @@
         <v>43308</v>
       </c>
       <c r="R21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="S21">
@@ -2591,8 +2713,8 @@
         <v>43374</v>
       </c>
       <c r="AL21">
-        <f t="shared" si="9"/>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="AM21">
         <v>15</v>
@@ -2600,9 +2722,9 @@
       <c r="AO21" s="1">
         <v>43374</v>
       </c>
-      <c r="AP21">
-        <f t="shared" si="10"/>
-        <v>7</v>
+      <c r="AP21" s="8">
+        <f t="shared" si="13"/>
+        <v>8</v>
       </c>
       <c r="AQ21">
         <v>4</v>
@@ -2611,8 +2733,8 @@
         <v>43374</v>
       </c>
       <c r="AT21">
-        <f t="shared" si="11"/>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="AU21">
         <v>8</v>
@@ -2621,8 +2743,8 @@
         <v>43374</v>
       </c>
       <c r="AX21">
-        <f t="shared" si="12"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="AY21">
         <v>7</v>
@@ -2633,7 +2755,7 @@
         <v>43311</v>
       </c>
       <c r="F22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="G22">
@@ -2643,7 +2765,7 @@
         <v>43311</v>
       </c>
       <c r="J22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="K22">
@@ -2653,7 +2775,7 @@
         <v>43311</v>
       </c>
       <c r="N22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O22">
@@ -2663,7 +2785,7 @@
         <v>43311</v>
       </c>
       <c r="R22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="S22">
@@ -2713,8 +2835,8 @@
         <v>43375</v>
       </c>
       <c r="AL22">
-        <f t="shared" si="9"/>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="AM22">
         <v>19</v>
@@ -2722,9 +2844,9 @@
       <c r="AO22" s="1">
         <v>43375</v>
       </c>
-      <c r="AP22">
-        <f t="shared" si="10"/>
-        <v>7</v>
+      <c r="AP22" s="8">
+        <f t="shared" si="13"/>
+        <v>8</v>
       </c>
       <c r="AQ22">
         <v>6</v>
@@ -2733,8 +2855,8 @@
         <v>43375</v>
       </c>
       <c r="AT22">
-        <f t="shared" si="11"/>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="AU22">
         <v>13</v>
@@ -2743,8 +2865,8 @@
         <v>43375</v>
       </c>
       <c r="AX22">
-        <f t="shared" si="12"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="AY22">
         <v>6</v>
@@ -2755,7 +2877,7 @@
         <v>43312</v>
       </c>
       <c r="F23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="G23">
@@ -2765,7 +2887,7 @@
         <v>43312</v>
       </c>
       <c r="J23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="K23">
@@ -2775,7 +2897,7 @@
         <v>43312</v>
       </c>
       <c r="R23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="S23">
@@ -2825,8 +2947,8 @@
         <v>43376</v>
       </c>
       <c r="AL23">
-        <f t="shared" si="9"/>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="AM23">
         <v>11</v>
@@ -2834,9 +2956,9 @@
       <c r="AO23" s="1">
         <v>43376</v>
       </c>
-      <c r="AP23">
-        <f t="shared" si="10"/>
-        <v>7</v>
+      <c r="AP23" s="8">
+        <f t="shared" si="13"/>
+        <v>8</v>
       </c>
       <c r="AQ23">
         <v>5</v>
@@ -2845,8 +2967,8 @@
         <v>43376</v>
       </c>
       <c r="AT23">
-        <f t="shared" si="11"/>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="AU23">
         <v>12</v>
@@ -2855,8 +2977,8 @@
         <v>43376</v>
       </c>
       <c r="AX23">
-        <f t="shared" si="12"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="AY23">
         <v>5</v>
@@ -2867,7 +2989,7 @@
         <v>43313</v>
       </c>
       <c r="F24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="G24">
@@ -2877,7 +2999,7 @@
         <v>43313</v>
       </c>
       <c r="J24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="K24">
@@ -2887,7 +3009,7 @@
         <v>43313</v>
       </c>
       <c r="N24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O24">
@@ -2897,7 +3019,7 @@
         <v>43313</v>
       </c>
       <c r="R24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="S24">
@@ -2947,8 +3069,8 @@
         <v>43377</v>
       </c>
       <c r="AL24">
-        <f t="shared" si="9"/>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
       <c r="AM24">
         <v>7</v>
@@ -2956,9 +3078,9 @@
       <c r="AO24" s="1">
         <v>43377</v>
       </c>
-      <c r="AP24">
-        <f t="shared" si="10"/>
-        <v>7</v>
+      <c r="AP24" s="8">
+        <f t="shared" si="13"/>
+        <v>9</v>
       </c>
       <c r="AQ24">
         <v>1</v>
@@ -2967,8 +3089,8 @@
         <v>43377</v>
       </c>
       <c r="AT24">
-        <f t="shared" si="11"/>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="AU24">
         <v>13</v>
@@ -2977,8 +3099,8 @@
         <v>43377</v>
       </c>
       <c r="AX24">
-        <f t="shared" si="12"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>9</v>
       </c>
       <c r="AY24">
         <v>5</v>
@@ -2989,7 +3111,7 @@
         <v>43314</v>
       </c>
       <c r="F25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="G25">
@@ -2999,7 +3121,7 @@
         <v>43314</v>
       </c>
       <c r="J25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="K25">
@@ -3009,7 +3131,7 @@
         <v>43314</v>
       </c>
       <c r="N25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O25">
@@ -3019,7 +3141,7 @@
         <v>43314</v>
       </c>
       <c r="R25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="S25">
@@ -3069,8 +3191,8 @@
         <v>43378</v>
       </c>
       <c r="AL25">
-        <f t="shared" si="9"/>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
       <c r="AM25">
         <v>17</v>
@@ -3078,9 +3200,9 @@
       <c r="AO25" s="1">
         <v>43378</v>
       </c>
-      <c r="AP25">
-        <f t="shared" si="10"/>
-        <v>7</v>
+      <c r="AP25" s="8">
+        <f t="shared" si="13"/>
+        <v>9</v>
       </c>
       <c r="AQ25">
         <v>6</v>
@@ -3089,8 +3211,8 @@
         <v>43378</v>
       </c>
       <c r="AT25">
-        <f t="shared" si="11"/>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="AU25">
         <v>12</v>
@@ -3099,8 +3221,8 @@
         <v>43378</v>
       </c>
       <c r="AX25">
-        <f t="shared" si="12"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>9</v>
       </c>
       <c r="AY25">
         <v>3</v>
@@ -3111,7 +3233,7 @@
         <v>43315</v>
       </c>
       <c r="F26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="G26">
@@ -3121,7 +3243,7 @@
         <v>43315</v>
       </c>
       <c r="J26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="K26">
@@ -3131,7 +3253,7 @@
         <v>43315</v>
       </c>
       <c r="N26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="O26">
@@ -3141,7 +3263,7 @@
         <v>43315</v>
       </c>
       <c r="R26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="S26">
@@ -3191,8 +3313,8 @@
         <v>43381</v>
       </c>
       <c r="AL26">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
       <c r="AM26">
         <v>25</v>
@@ -3200,9 +3322,9 @@
       <c r="AO26" s="1">
         <v>43381</v>
       </c>
-      <c r="AP26">
-        <f t="shared" si="10"/>
-        <v>8</v>
+      <c r="AP26" s="8">
+        <f t="shared" si="13"/>
+        <v>9</v>
       </c>
       <c r="AQ26">
         <v>7</v>
@@ -3211,8 +3333,8 @@
         <v>43381</v>
       </c>
       <c r="AT26">
-        <f t="shared" si="11"/>
-        <v>8</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="AU26">
         <v>13</v>
@@ -3221,8 +3343,8 @@
         <v>43381</v>
       </c>
       <c r="AX26">
-        <f t="shared" si="12"/>
-        <v>8</v>
+        <f t="shared" si="7"/>
+        <v>9</v>
       </c>
       <c r="AY26">
         <v>4</v>
@@ -3233,7 +3355,7 @@
         <v>43319</v>
       </c>
       <c r="F27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="G27">
@@ -3313,8 +3435,8 @@
         <v>43382</v>
       </c>
       <c r="AL27">
-        <f t="shared" si="9"/>
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>10</v>
       </c>
       <c r="AM27">
         <v>13</v>
@@ -3322,9 +3444,9 @@
       <c r="AO27" s="1">
         <v>43382</v>
       </c>
-      <c r="AP27">
-        <f t="shared" si="10"/>
-        <v>8</v>
+      <c r="AP27" s="8">
+        <f t="shared" si="13"/>
+        <v>10</v>
       </c>
       <c r="AQ27">
         <v>6</v>

</xml_diff>